<commit_message>
Modelo de arquivo para lista de materiais do projeto semestral.
</commit_message>
<xml_diff>
--- a/1.3-laboratorio/modelos-de-arquivo/ete103-lista-de-materiais-projeto-semestral.xlsx
+++ b/1.3-laboratorio/modelos-de-arquivo/ete103-lista-de-materiais-projeto-semestral.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>ETE103 - Fundamentos de Circuitos Analógicos</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>2 - Noturno</t>
+  </si>
+  <si>
+    <t>Observações</t>
   </si>
 </sst>
 </file>
@@ -280,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -288,25 +291,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -337,32 +328,51 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,13 +412,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>238125</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>47626</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>2886075</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>257176</xdr:rowOff>
+          <xdr:rowOff>257175</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -455,9 +465,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>238124</xdr:colOff>
+          <xdr:colOff>238125</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>95251</xdr:rowOff>
+          <xdr:rowOff>95250</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -772,9 +782,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -788,77 +798,77 @@
   <sheetData>
     <row r="1" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="4" spans="2:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="6" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:4" s="13" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:4" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
     </row>
     <row r="10" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
     </row>
     <row r="12" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
     </row>
     <row r="14" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="24">
+      <c r="C14" s="21"/>
+      <c r="D14" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="28"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
     </row>
     <row r="16" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
     </row>
     <row r="17" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
@@ -866,231 +876,249 @@
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="24">
+      <c r="C18" s="27"/>
+      <c r="D18" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
+    <row r="20" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B21" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+    </row>
+    <row r="22" spans="2:4" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="2:4" s="1" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="30"/>
+    </row>
+    <row r="24" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-    </row>
-    <row r="23" spans="2:4" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+    </row>
+    <row r="27" spans="2:4" s="3" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C27" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-    </row>
-    <row r="25" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-    </row>
-    <row r="26" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-    </row>
-    <row r="27" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
+      <c r="D27" s="29"/>
     </row>
     <row r="28" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
     </row>
     <row r="29" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="19"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
     </row>
     <row r="30" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
     </row>
     <row r="31" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="19"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
     </row>
     <row r="32" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
     </row>
     <row r="33" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="19"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
     </row>
     <row r="34" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
     </row>
     <row r="35" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="19"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
     </row>
     <row r="36" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
     </row>
     <row r="37" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
     </row>
     <row r="38" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
     </row>
     <row r="39" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="19"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
     </row>
     <row r="40" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
     </row>
     <row r="41" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="19"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
     </row>
     <row r="42" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
     </row>
     <row r="43" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="19"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
     </row>
     <row r="44" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="19"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
     </row>
     <row r="45" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
     </row>
     <row r="46" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="19"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
     </row>
     <row r="47" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="19"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
     </row>
     <row r="48" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="19"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
     </row>
     <row r="49" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="19"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
     </row>
     <row r="50" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="19"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
     </row>
     <row r="51" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="19"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
     </row>
     <row r="52" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="19"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="24"/>
     </row>
     <row r="53" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="19"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
     </row>
     <row r="54" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="19"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
     </row>
     <row r="55" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="19"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
+    </row>
+    <row r="56" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="15"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+    </row>
+    <row r="57" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="15"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+    </row>
+    <row r="58" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="15"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+    </row>
+    <row r="59" spans="2:4" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="15"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="24"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatRows="0"/>
-  <mergeCells count="37">
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
+  <mergeCells count="38">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
     <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="C45:D45"/>
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1187,12 +1215,12 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1202,7 +1230,7 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>